<commit_message>
Linking, shapes and key.
</commit_message>
<xml_diff>
--- a/books.xlsx
+++ b/books.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jennie\Documents\personal\repos\BookOfMagnus\src\bookofmagnus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jennie\Documents\personal\repos\BookOfMagnus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254284A4-1B73-45CF-A796-93CDBF12F21F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDEF364-C006-48D3-94F6-B94EFBA8B28F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{081CEC6C-671A-4C6D-9320-71B970466DA2}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="19200" windowHeight="11770" xr2:uid="{081CEC6C-671A-4C6D-9320-71B970466DA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="63">
   <si>
     <t>Title</t>
   </si>
@@ -205,6 +205,21 @@
   </si>
   <si>
     <t>A Thousand Sons,Tales of Heresy</t>
+  </si>
+  <si>
+    <t>Legion,Fulgrim</t>
+  </si>
+  <si>
+    <t>The First Heretic,Battle for the Abyss</t>
+  </si>
+  <si>
+    <t>Know No Fear,Betrayer</t>
+  </si>
+  <si>
+    <t>Battle for the Abyss,Vulkan Lives,Fallen Angels</t>
+  </si>
+  <si>
+    <t>Fulgrim,Legion</t>
   </si>
 </sst>
 </file>
@@ -599,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EFFEC2-FF66-493C-91A3-F32744CC455D}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -725,7 +740,7 @@
       <c r="C9" s="4">
         <v>2008</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
@@ -860,7 +875,7 @@
         <v>2011</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -899,7 +914,9 @@
       <c r="C22" s="4">
         <v>2012</v>
       </c>
-      <c r="D22" s="4"/>
+      <c r="D22" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
@@ -935,7 +952,9 @@
       <c r="C25" s="4">
         <v>2012</v>
       </c>
-      <c r="D25" s="4"/>
+      <c r="D25" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
@@ -973,7 +992,9 @@
       <c r="C28" s="4">
         <v>2013</v>
       </c>
-      <c r="D28" s="4"/>
+      <c r="D28" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
@@ -985,7 +1006,9 @@
       <c r="C29" s="4">
         <v>2013</v>
       </c>
-      <c r="D29" s="4"/>
+      <c r="D29" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
@@ -997,7 +1020,9 @@
       <c r="C30" s="4">
         <v>2013</v>
       </c>
-      <c r="D30" s="4"/>
+      <c r="D30" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
@@ -1009,7 +1034,9 @@
       <c r="C31" s="4">
         <v>2013</v>
       </c>
-      <c r="D31" s="4"/>
+      <c r="D31" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
@@ -1033,7 +1060,9 @@
       <c r="C33" s="4">
         <v>2013</v>
       </c>
-      <c r="D33" s="4"/>
+      <c r="D33" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
@@ -1069,7 +1098,9 @@
       <c r="C36" s="4">
         <v>2014</v>
       </c>
-      <c r="D36" s="4"/>
+      <c r="D36" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
@@ -1141,7 +1172,9 @@
       <c r="C42" s="4">
         <v>2015</v>
       </c>
-      <c r="D42" s="4"/>
+      <c r="D42" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
@@ -1201,7 +1234,9 @@
       <c r="C47" s="4">
         <v>2016</v>
       </c>
-      <c r="D47" s="4"/>
+      <c r="D47" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
@@ -1249,7 +1284,9 @@
       <c r="C51" s="4">
         <v>2016</v>
       </c>
-      <c r="D51" s="4"/>
+      <c r="D51" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Links and working on style.
</commit_message>
<xml_diff>
--- a/books.xlsx
+++ b/books.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jennie\Documents\personal\repos\BookOfMagnus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDEF364-C006-48D3-94F6-B94EFBA8B28F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E27743-0F62-45CF-BE1D-9E5DCA4A9929}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="19200" windowHeight="11770" xr2:uid="{081CEC6C-671A-4C6D-9320-71B970466DA2}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="19200" windowHeight="9980" xr2:uid="{081CEC6C-671A-4C6D-9320-71B970466DA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="64">
   <si>
     <t>Title</t>
   </si>
@@ -216,10 +216,13 @@
     <t>Know No Fear,Betrayer</t>
   </si>
   <si>
-    <t>Battle for the Abyss,Vulkan Lives,Fallen Angels</t>
-  </si>
-  <si>
     <t>Fulgrim,Legion</t>
+  </si>
+  <si>
+    <t>The Flight of the Eisenstein,Nemesis</t>
+  </si>
+  <si>
+    <t>Betrayer,Battle for the Abyss,Vulkan Lives,Fallen Angels</t>
   </si>
 </sst>
 </file>
@@ -614,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EFFEC2-FF66-493C-91A3-F32744CC455D}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -967,7 +970,7 @@
         <v>2012</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -1007,7 +1010,7 @@
         <v>2013</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -1035,7 +1038,7 @@
         <v>2013</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -1210,7 +1213,9 @@
       <c r="C45" s="4">
         <v>2015</v>
       </c>
-      <c r="D45" s="4"/>
+      <c r="D45" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
@@ -1260,7 +1265,9 @@
       <c r="C49" s="4">
         <v>2016</v>
       </c>
-      <c r="D49" s="4"/>
+      <c r="D49" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">

</xml_diff>